<commit_message>
file name must be added as argument when running the script; the script can now go to the next page for more than 20 entries on the page; added wait time for manual cloudflare verification
</commit_message>
<xml_diff>
--- a/Baza de date - Cautare ANI_short.xlsx
+++ b/Baza de date - Cautare ANI_short.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Alba" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Arad" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Iasi" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Nr</t>
   </si>
@@ -56,40 +56,32 @@
     <t>Nume complet: DÎRLĂU E. Andrei-Emil</t>
   </si>
   <si>
-    <t>VARGA Glad-Aurel</t>
+    <t>CHIRICA MIHAI</t>
   </si>
   <si>
-    <t>Partidul Naţional Liberal</t>
+    <t>Primar</t>
+  </si>
+  <si>
+    <t>PNL</t>
+  </si>
+  <si>
+    <t>Iasi</t>
   </si>
   <si>
     <t>Incarcat</t>
   </si>
   <si>
-    <t>Patricia Herrmann</t>
+    <t>Emanuel Toarcăş-Marcu</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">FYI </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>Figureaza in ANI ca ”Varga A. Glad Aurel” | Membru în Cam. Deputaților, nu in Senat |  Arondat la Sectorul 5</t>
-    </r>
+    <t>Numele greşit la Declarația de Avere din 07.06.2021, Lipseşte funcția şi Instituția în Declarația de Interese din 15.07.2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -106,6 +98,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -212,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -249,8 +245,23 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -301,7 +312,7 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="Arad-style">
+    <tableStyle count="3" pivot="0" name="Iasi-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -346,7 +357,7 @@
     <tableColumn name="Cine lucrează" id="7"/>
     <tableColumn name="Observatii/Comentarii" id="8"/>
   </tableColumns>
-  <tableStyleInfo name="Arad-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Iasi-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -654,9 +665,10 @@
     </row>
     <row r="3">
       <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -26214,34 +26226,6 @@
       <c r="X915" s="11"/>
       <c r="Y915" s="11"/>
       <c r="Z915" s="11"/>
-    </row>
-    <row r="916">
-      <c r="A916" s="11"/>
-      <c r="B916" s="11"/>
-      <c r="C916" s="11"/>
-      <c r="D916" s="11"/>
-      <c r="E916" s="11"/>
-      <c r="F916" s="11"/>
-      <c r="G916" s="11"/>
-      <c r="H916" s="11"/>
-      <c r="I916" s="11"/>
-      <c r="J916" s="11"/>
-      <c r="K916" s="11"/>
-      <c r="L916" s="11"/>
-      <c r="M916" s="11"/>
-      <c r="N916" s="11"/>
-      <c r="O916" s="11"/>
-      <c r="P916" s="11"/>
-      <c r="Q916" s="11"/>
-      <c r="R916" s="11"/>
-      <c r="S916" s="11"/>
-      <c r="T916" s="11"/>
-      <c r="U916" s="11"/>
-      <c r="V916" s="11"/>
-      <c r="W916" s="11"/>
-      <c r="X916" s="11"/>
-      <c r="Y916" s="11"/>
-      <c r="Z916" s="11"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -26326,48 +26310,56 @@
       <c r="Y1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="6">
-        <v>3.0</v>
+      <c r="A2" s="12">
+        <v>74.0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
+      <c r="G2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
     </row>
   </sheetData>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2">
+      <formula1>"Senat,Camera Deputatilor,Presedinte CJ,Consilier judetean,Consilier local,Primar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2">
+      <formula1>"Incarcat,In lucru"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2">
       <formula1>"Senat,Camera Deputatilor,Presedinte CJ,Consilier judetean,Consilier local,Primar"</formula1>
     </dataValidation>

</xml_diff>